<commit_message>
Backup medical form ready
</commit_message>
<xml_diff>
--- a/Parabit Project Data File/Bank Jammu-1.xlsx
+++ b/Parabit Project Data File/Bank Jammu-1.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Parabit ki backchodiya\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ParabitProjectFile\Parabit Project Data File\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6FAB57-EB3F-43D2-B968-6B6E04C4D00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9192"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -174,7 +184,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -305,6 +315,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -340,6 +367,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -515,11 +559,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="E35" sqref="E35:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,6 +629,9 @@
       <c r="D3" t="s">
         <v>19</v>
       </c>
+      <c r="E3">
+        <v>91859314288</v>
+      </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
@@ -602,6 +649,9 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
+      <c r="E4">
+        <v>43926050845</v>
+      </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
@@ -619,6 +669,9 @@
       <c r="D5" t="s">
         <v>21</v>
       </c>
+      <c r="E5">
+        <v>21888236206</v>
+      </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
@@ -636,7 +689,9 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>85085131239</v>
+      </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
@@ -654,7 +709,9 @@
       <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>43930291095</v>
+      </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
@@ -672,7 +729,9 @@
       <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>61772075081</v>
+      </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
@@ -690,7 +749,9 @@
       <c r="D9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>37593250969</v>
+      </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
@@ -708,7 +769,9 @@
       <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>86519645201</v>
+      </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
@@ -726,7 +789,9 @@
       <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>65816953840</v>
+      </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
@@ -744,7 +809,9 @@
       <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>19027838196</v>
+      </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
@@ -762,6 +829,9 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
+      <c r="E13">
+        <v>93007426639</v>
+      </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
@@ -779,6 +849,9 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
+      <c r="E14">
+        <v>52689747707</v>
+      </c>
       <c r="F14" t="s">
         <v>14</v>
       </c>
@@ -796,6 +869,9 @@
       <c r="D15" t="s">
         <v>31</v>
       </c>
+      <c r="E15">
+        <v>27170230129</v>
+      </c>
       <c r="F15" t="s">
         <v>14</v>
       </c>
@@ -813,6 +889,9 @@
       <c r="D16" t="s">
         <v>32</v>
       </c>
+      <c r="E16">
+        <v>62475902271</v>
+      </c>
       <c r="F16" t="s">
         <v>13</v>
       </c>
@@ -830,6 +909,9 @@
       <c r="D17" t="s">
         <v>33</v>
       </c>
+      <c r="E17">
+        <v>79155748042</v>
+      </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
@@ -847,6 +929,9 @@
       <c r="D18" t="s">
         <v>34</v>
       </c>
+      <c r="E18">
+        <v>99299269119</v>
+      </c>
       <c r="F18" t="s">
         <v>13</v>
       </c>
@@ -864,6 +949,9 @@
       <c r="D19" t="s">
         <v>35</v>
       </c>
+      <c r="E19">
+        <v>36529164009</v>
+      </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
@@ -881,6 +969,9 @@
       <c r="D20" t="s">
         <v>36</v>
       </c>
+      <c r="E20">
+        <v>60906578690</v>
+      </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
@@ -898,6 +989,9 @@
       <c r="D21" t="s">
         <v>37</v>
       </c>
+      <c r="E21">
+        <v>54817896850</v>
+      </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
@@ -915,6 +1009,9 @@
       <c r="D22" t="s">
         <v>38</v>
       </c>
+      <c r="E22">
+        <v>62996019533</v>
+      </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
@@ -932,6 +1029,9 @@
       <c r="D23" t="s">
         <v>39</v>
       </c>
+      <c r="E23">
+        <v>68037271812</v>
+      </c>
       <c r="F23" t="s">
         <v>13</v>
       </c>
@@ -949,6 +1049,9 @@
       <c r="D24" t="s">
         <v>40</v>
       </c>
+      <c r="E24">
+        <v>14267205350</v>
+      </c>
       <c r="F24" t="s">
         <v>13</v>
       </c>
@@ -966,6 +1069,9 @@
       <c r="D25" t="s">
         <v>41</v>
       </c>
+      <c r="E25">
+        <v>66682159518</v>
+      </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
@@ -983,6 +1089,9 @@
       <c r="D26" t="s">
         <v>42</v>
       </c>
+      <c r="E26">
+        <v>34729008256</v>
+      </c>
       <c r="F26" t="s">
         <v>14</v>
       </c>
@@ -1000,6 +1109,9 @@
       <c r="D27" t="s">
         <v>43</v>
       </c>
+      <c r="E27">
+        <v>38777031370</v>
+      </c>
       <c r="F27" t="s">
         <v>13</v>
       </c>
@@ -1017,6 +1129,9 @@
       <c r="D28" t="s">
         <v>44</v>
       </c>
+      <c r="E28">
+        <v>90705678790</v>
+      </c>
       <c r="F28" t="s">
         <v>13</v>
       </c>
@@ -1034,6 +1149,9 @@
       <c r="D29" t="s">
         <v>46</v>
       </c>
+      <c r="E29">
+        <v>34602836341</v>
+      </c>
       <c r="F29" t="s">
         <v>13</v>
       </c>
@@ -1051,6 +1169,9 @@
       <c r="D30" t="s">
         <v>47</v>
       </c>
+      <c r="E30">
+        <v>26046347589</v>
+      </c>
       <c r="F30" t="s">
         <v>13</v>
       </c>
@@ -1068,6 +1189,9 @@
       <c r="D31" t="s">
         <v>48</v>
       </c>
+      <c r="E31">
+        <v>83702032370</v>
+      </c>
       <c r="F31" t="s">
         <v>13</v>
       </c>
@@ -1085,6 +1209,9 @@
       <c r="D32" t="s">
         <v>49</v>
       </c>
+      <c r="E32">
+        <v>94338333262</v>
+      </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
@@ -1102,6 +1229,9 @@
       <c r="D33" t="s">
         <v>49</v>
       </c>
+      <c r="E33">
+        <v>98667204125</v>
+      </c>
       <c r="F33" t="s">
         <v>14</v>
       </c>
@@ -1118,6 +1248,9 @@
       </c>
       <c r="D34" t="s">
         <v>45</v>
+      </c>
+      <c r="E34">
+        <v>50944537481</v>
       </c>
       <c r="F34" t="s">
         <v>13</v>
@@ -1127,4 +1260,226 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB000F22-5659-43BA-997E-E2B6B7A1CE63}">
+  <dimension ref="A1:A34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <f ca="1">RANDBETWEEN(11111111111,99999999999)</f>
+        <v>82573189301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f t="shared" ref="A2:A34" ca="1" si="0">RANDBETWEEN(11111111111,99999999999)</f>
+        <v>99752330450</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f t="shared" ca="1" si="0"/>
+        <v>47237889697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ca="1" si="0"/>
+        <v>29044118843</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>89732309605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>32775871480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>73226073386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>45137611795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>59144783758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>12826481060</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>51441604662</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>39265746304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>49825333593</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" ca="1" si="0"/>
+        <v>25576705634</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" ca="1" si="0"/>
+        <v>84435026029</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" ca="1" si="0"/>
+        <v>56360244022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" ca="1" si="0"/>
+        <v>74154583392</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" ca="1" si="0"/>
+        <v>46837862754</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" ca="1" si="0"/>
+        <v>97617500354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" ca="1" si="0"/>
+        <v>90288768986</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" ca="1" si="0"/>
+        <v>86611648864</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" ca="1" si="0"/>
+        <v>71817061756</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" ca="1" si="0"/>
+        <v>11835960787</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" ca="1" si="0"/>
+        <v>23729259853</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" ca="1" si="0"/>
+        <v>78623832822</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" ca="1" si="0"/>
+        <v>86453890277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" ca="1" si="0"/>
+        <v>52341000257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" ca="1" si="0"/>
+        <v>70177020088</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" ca="1" si="0"/>
+        <v>81065001380</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" ca="1" si="0"/>
+        <v>28437470163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" ca="1" si="0"/>
+        <v>99961378695</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" ca="1" si="0"/>
+        <v>52297928999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" ca="1" si="0"/>
+        <v>32428614009</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" ca="1" si="0"/>
+        <v>86029167166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>